<commit_message>
Change SI units from g/kWh to kg/MWh
Change units to match those shown on the website.
</commit_message>
<xml_diff>
--- a/Calculated values/2017/2017 Q1 US Power Sector CO2 Emissions Intensity.xlsx
+++ b/Calculated values/2017/2017 Q1 US Power Sector CO2 Emissions Intensity.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Monthly" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t>quarter</t>
-  </si>
-  <si>
-    <t>index (g/kWh)</t>
   </si>
   <si>
     <t>change since 2005</t>
@@ -243,6 +240,9 @@
   </si>
   <si>
     <t>2016 Q4</t>
+  </si>
+  <si>
+    <t>index (kg/MWh)</t>
   </si>
 </sst>
 </file>
@@ -616,7 +616,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -648,13 +650,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -6234,7 +6236,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6260,16 +6264,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -6289,7 +6293,7 @@
         <v>637.93666910125739</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G2">
         <v>6.1897338208549167E-2</v>
@@ -6315,7 +6319,7 @@
         <v>628.18870766423856</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3">
         <v>4.5671065595135812E-2</v>
@@ -6341,7 +6345,7 @@
         <v>640.59782791486873</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G4">
         <v>6.6327052939801845E-2</v>
@@ -6367,7 +6371,7 @@
         <v>616.64584616171044</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G5">
         <v>2.6457036211759839E-2</v>
@@ -6393,7 +6397,7 @@
         <v>607.49371275566637</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G6">
         <v>1.122256769233829E-2</v>
@@ -6419,7 +6423,7 @@
         <v>606.00127878425394</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G7">
         <v>8.7382902735036096E-3</v>
@@ -6445,7 +6449,7 @@
         <v>628.02546510332206</v>
       </c>
       <c r="F8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G8">
         <v>4.5399335109468947E-2</v>
@@ -6471,7 +6475,7 @@
         <v>626.09681437748031</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G9">
         <v>4.2188939514886413E-2</v>
@@ -6497,7 +6501,7 @@
         <v>625.75914237916231</v>
       </c>
       <c r="F10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G10">
         <v>4.162685708011022E-2</v>
@@ -6523,7 +6527,7 @@
         <v>602.35551785165978</v>
       </c>
       <c r="F11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G11">
         <v>2.6696254395466262E-3</v>
@@ -6549,7 +6553,7 @@
         <v>624.58290028365673</v>
       </c>
       <c r="F12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G12">
         <v>3.9668906689727543E-2</v>
@@ -6575,7 +6579,7 @@
         <v>625.64736056792356</v>
       </c>
       <c r="F13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G13">
         <v>4.1440787187025381E-2</v>
@@ -6601,7 +6605,7 @@
         <v>607.92553540867118</v>
       </c>
       <c r="F14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G14">
         <v>1.194137152979443E-2</v>
@@ -6627,7 +6631,7 @@
         <v>592.72419815409557</v>
       </c>
       <c r="F15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G15">
         <v>-1.3362487536005861E-2</v>
@@ -6653,7 +6657,7 @@
         <v>602.64053519008417</v>
       </c>
       <c r="F16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G16">
         <v>3.1440599213307359E-3</v>
@@ -6679,7 +6683,7 @@
         <v>606.29491210156164</v>
       </c>
       <c r="F17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G17">
         <v>9.2270667511086223E-3</v>
@@ -6705,7 +6709,7 @@
         <v>603.62768682337617</v>
       </c>
       <c r="F18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G18">
         <v>4.7872538974315388E-3</v>
@@ -6731,7 +6735,7 @@
         <v>586.79842656595088</v>
       </c>
       <c r="F19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G19">
         <v>-2.3226415071552351E-2</v>
@@ -6757,7 +6761,7 @@
         <v>605.28330150549129</v>
       </c>
       <c r="F20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G20">
         <v>7.5431588472346248E-3</v>
@@ -6783,7 +6787,7 @@
         <v>606.42617084845836</v>
       </c>
       <c r="F21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G21">
         <v>9.4455575836587934E-3</v>
@@ -6809,7 +6813,7 @@
         <v>586.76592791474536</v>
       </c>
       <c r="F22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G22">
         <v>-2.3280511712930749E-2</v>
@@ -6835,7 +6839,7 @@
         <v>569.31877171183305</v>
       </c>
       <c r="F23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G23">
         <v>-5.2322718609867452E-2</v>
@@ -6861,7 +6865,7 @@
         <v>594.45604223797125</v>
       </c>
       <c r="F24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G24">
         <v>-1.04796925628768E-2</v>
@@ -6887,7 +6891,7 @@
         <v>597.57077771136153</v>
       </c>
       <c r="F25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G25">
         <v>-5.2949626851028489E-3</v>
@@ -6913,7 +6917,7 @@
         <v>585.70154241269745</v>
       </c>
       <c r="F26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G26">
         <v>-2.5052267729158511E-2</v>
@@ -6939,7 +6943,7 @@
         <v>582.5720592871844</v>
       </c>
       <c r="F27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G27">
         <v>-3.0261546270291251E-2</v>
@@ -6965,7 +6969,7 @@
         <v>595.35035190232702</v>
       </c>
       <c r="F28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G28">
         <v>-8.9910415758572143E-3</v>
@@ -6991,7 +6995,7 @@
         <v>594.71472678759858</v>
       </c>
       <c r="F29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G29">
         <v>-1.004909114428781E-2</v>
@@ -7017,7 +7021,7 @@
         <v>587.92309062976744</v>
       </c>
       <c r="F30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G30">
         <v>-2.1354320499173941E-2</v>
@@ -7043,7 +7047,7 @@
         <v>571.95090942783384</v>
       </c>
       <c r="F31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G31">
         <v>-4.7941311849918497E-2</v>
@@ -7069,7 +7073,7 @@
         <v>587.84839993191372</v>
       </c>
       <c r="F32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G32">
         <v>-2.147864922501996E-2</v>
@@ -7095,7 +7099,7 @@
         <v>579.05499134967499</v>
       </c>
       <c r="F33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G33">
         <v>-3.6115991173735207E-2</v>
@@ -7121,7 +7125,7 @@
         <v>556.4480200307122</v>
       </c>
       <c r="F34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G34">
         <v>-7.3747128920346183E-2</v>
@@ -7147,7 +7151,7 @@
         <v>534.08353834024376</v>
       </c>
       <c r="F35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G35">
         <v>-0.1109746230084039</v>
@@ -7173,7 +7177,7 @@
         <v>556.3079868525831</v>
       </c>
       <c r="F36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G36">
         <v>-7.3980225505506703E-2</v>
@@ -7199,7 +7203,7 @@
         <v>560.18661879147692</v>
       </c>
       <c r="F37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G37">
         <v>-6.7523927989948371E-2</v>
@@ -7225,7 +7229,7 @@
         <v>563.71082785479609</v>
       </c>
       <c r="F38" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G38">
         <v>-6.1657596103271588E-2</v>
@@ -7251,7 +7255,7 @@
         <v>550.20586790387824</v>
       </c>
       <c r="F39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G39">
         <v>-8.4137697528851266E-2</v>
@@ -7277,7 +7281,7 @@
         <v>571.20065025742167</v>
       </c>
       <c r="F40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G40">
         <v>-4.9190179103700361E-2</v>
@@ -7303,7 +7307,7 @@
         <v>550.99879177484183</v>
       </c>
       <c r="F41" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G41">
         <v>-8.2817811419835935E-2</v>
@@ -7329,7 +7333,7 @@
         <v>542.86833357955345</v>
       </c>
       <c r="F42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G42">
         <v>-9.6351618667749786E-2</v>
@@ -7355,7 +7359,7 @@
         <v>536.58073054746262</v>
       </c>
       <c r="F43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G43">
         <v>-0.10681784399525091</v>
@@ -7381,7 +7385,7 @@
         <v>558.3245998947375</v>
       </c>
       <c r="F44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G44">
         <v>-7.0623409499495762E-2</v>
@@ -7407,7 +7411,7 @@
         <v>518.226499558829</v>
       </c>
       <c r="F45" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G45">
         <v>-0.1373699504592881</v>
@@ -7433,7 +7437,7 @@
         <v>493.72035489025421</v>
       </c>
       <c r="F46" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G46">
         <v>-0.1781624163164007</v>
@@ -7459,7 +7463,7 @@
         <v>497.69807672822151</v>
       </c>
       <c r="F47" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G47">
         <v>-0.17154117562518559</v>
@@ -7485,7 +7489,7 @@
         <v>540.56543443479518</v>
       </c>
       <c r="F48" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G48">
         <v>-0.1001849811164498</v>
@@ -7511,7 +7515,7 @@
         <v>523.3752960549192</v>
       </c>
       <c r="F49" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G49">
         <v>-0.12879936099642109</v>
@@ -7537,7 +7541,7 @@
         <v>513.87963369867134</v>
       </c>
       <c r="F50" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G50">
         <v>-0.14460566132217689</v>
@@ -7563,7 +7567,7 @@
         <v>503.59466237043779</v>
       </c>
       <c r="F51" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G51">
         <v>-0.16172583046434119</v>
@@ -7589,7 +7593,7 @@
         <v>534.58261927447609</v>
       </c>
       <c r="F52" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G52">
         <v>-0.1101438623055294</v>
@@ -7615,7 +7619,7 @@
         <v>513.84413789304506</v>
       </c>
       <c r="F53" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G53">
         <v>-0.14466474697023221</v>
@@ -7641,7 +7645,7 @@
         <v>529.81519615357854</v>
       </c>
       <c r="F54" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G54">
         <v>-0.11807962484654649</v>
@@ -7667,7 +7671,7 @@
         <v>495.54620598249971</v>
       </c>
       <c r="F55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G55">
         <v>-0.1751231390515397</v>
@@ -7693,7 +7697,7 @@
         <v>525.21849439541586</v>
       </c>
       <c r="F56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G56">
         <v>-0.1257312078295538</v>
@@ -7719,7 +7723,7 @@
         <v>490.99772867588979</v>
       </c>
       <c r="F57" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G57">
         <v>-0.182694448522738</v>
@@ -7745,7 +7749,7 @@
         <v>488.72432920132889</v>
       </c>
       <c r="F58" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G58">
         <v>-0.18647870637723929</v>
@@ -7771,7 +7775,7 @@
         <v>474.56747720666681</v>
       </c>
       <c r="F59" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G59">
         <v>-0.21004393499424809</v>
@@ -7797,7 +7801,7 @@
         <v>509.13770456339859</v>
       </c>
       <c r="F60" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G60">
         <v>-0.15249898705592679</v>
@@ -7823,7 +7827,7 @@
         <v>450.39472908731682</v>
       </c>
       <c r="F61" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G61">
         <v>-0.25028143524844509</v>
@@ -7849,7 +7853,7 @@
         <v>429.7474796111826</v>
       </c>
       <c r="F62" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G62">
         <v>-0.28465045700561048</v>
@@ -7875,7 +7879,7 @@
         <v>434.3286446295146</v>
       </c>
       <c r="F63" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G63">
         <v>-0.27702473618646639</v>
@@ -7901,7 +7905,7 @@
         <v>497.07099226263722</v>
       </c>
       <c r="F64" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G64">
         <v>-0.1725850085902573</v>
@@ -7927,7 +7931,7 @@
         <v>453.92603105033641</v>
       </c>
       <c r="F65" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G65">
         <v>-0.24440329665480681</v>
@@ -7945,7 +7949,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7967,13 +7973,13 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>